<commit_message>
[PSR-2047] Tangible moveable property acquired from arms length template update
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Tangible moveable property acquired from an arm's length party.xlsx
+++ b/conf/TEMPLATE - SIPP Tangible moveable property acquired from an arm's length party.xlsx
@@ -4,20 +4,19 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Tangible moveable property" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="RqXK7YJeIaRWN07x2DPFwbdb/OmhfZmKXoosMwdX9Q0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="TIxFkKUvKwL/3Xl4/40TyWaRID+0vtL9W1VIsBpJUXU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -60,7 +59,8 @@
     <t>Description of asset</t>
   </si>
   <si>
-    <t>What is the date the scheme acquired the Tangible Moveable Property?</t>
+    <t xml:space="preserve">What is the date the scheme acquired the Tangible Moveable Property?
+</t>
   </si>
   <si>
     <t>What is the total cost of the Tangible Moveable Property at the date the scheme acquired it?</t>
@@ -201,7 +201,7 @@
 Mandatory question</t>
   </si>
   <si>
-    <t>Enter amount as whole number and to two decimal places.
+    <t>Enter amount to two decimal places.
 Enter the total amount in GBP (pounds and pence).
 Enter the total amount received in respect of the relevant member for this tangible movable property
 If multiple tangible movable properties for this member - enter each tangible movable property on a separate row</t>
@@ -242,14 +242,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="dd-mm-yyyy"/>
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="d-m-yyyy"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="168" formatCode="yyyy-mm-dd"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -295,11 +292,25 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
+      <i/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +327,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -339,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -348,9 +365,6 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -367,34 +381,25 @@
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +410,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -653,7 +654,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -692,71 +693,71 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="U2" s="9"/>
@@ -764,24 +765,24 @@
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
@@ -790,25 +791,25 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
@@ -817,25 +818,25 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -844,25 +845,25 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
@@ -871,25 +872,25 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -898,25 +899,25 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -925,25 +926,25 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -952,25 +953,25 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -979,25 +980,25 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -1006,25 +1007,25 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -7433,89 +7434,4 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="9">
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="E15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="E17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="E21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="E22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>